<commit_message>
README added email automation finished sms added
</commit_message>
<xml_diff>
--- a/csv_excel/res/excel_writer.xlsx
+++ b/csv_excel/res/excel_writer.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="woop woop" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -589,6 +590,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -640,4 +642,22 @@
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
 </file>
</xml_diff>